<commit_message>
Intégration des tableaux de la cartographie
</commit_message>
<xml_diff>
--- a/Toolbox Cybersecurite.xlsx
+++ b/Toolbox Cybersecurite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bforsecurity/Downloads/c8e7b9c8-f48b-42a9-9309-d8b84f9210b5_Export-6f5f6938-2ec2-46c4-87ff-75b67db0e793/Toolbox Cybersécurité - V1 0 -19 01 2024 d1e4f3c3c9bc4992affa2afa2050d6f3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bforsecurity/Library/Mobile Documents/com~apple~CloudDocs/3-MISSIONS/Toolbox guide hygiene/Toolbox-Cybersecurite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D9974-8662-684B-8CFE-A7423055290A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF2630A-2040-2C47-A5F4-E22768EF8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="38020" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="144">
   <si>
     <t>Etat</t>
   </si>
@@ -330,13 +330,206 @@
   </si>
   <si>
     <t>OBJ-10'!A1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Système d'exploitation</t>
+  </si>
+  <si>
+    <t>Entités tierces liées</t>
+  </si>
+  <si>
+    <t>Logiciels liés</t>
+  </si>
+  <si>
+    <t>Règles de sauvegarde</t>
+  </si>
+  <si>
+    <t>Support/Maintenance/Garantie</t>
+  </si>
+  <si>
+    <t>Données chiffrées</t>
+  </si>
+  <si>
+    <t>MATERIEL</t>
+  </si>
+  <si>
+    <t>LOGICIEL</t>
+  </si>
+  <si>
+    <t>Localisation</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t>Sensible</t>
+  </si>
+  <si>
+    <t>Type d'authentification</t>
+  </si>
+  <si>
+    <t>Profil</t>
+  </si>
+  <si>
+    <t>Matériel lié</t>
+  </si>
+  <si>
+    <t>Exigences de sécurité</t>
+  </si>
+  <si>
+    <t>Mise à jour</t>
+  </si>
+  <si>
+    <t>INTERCONNEXION</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Protocole</t>
+  </si>
+  <si>
+    <t>Données sensibles</t>
+  </si>
+  <si>
+    <t>ENTITE TIERCE</t>
+  </si>
+  <si>
+    <t>ColoContact sécuriténne4</t>
+  </si>
+  <si>
+    <t>Logiciel lié</t>
+  </si>
+  <si>
+    <t>A propos</t>
+  </si>
+  <si>
+    <t>Destinée à toutes les entités (startup, petite ou grande entreprise, association, …) souhaitant intégrer la cybersécurité à leurs activités.</t>
+  </si>
+  <si>
+    <t>Ce template vous présente des actions simples et concrètes sur les mesures de cybersécurité à mettre en place.</t>
+  </si>
+  <si>
+    <t>La mise en oeuvre de ces actions doit se faire par une personne compétente afin d’en maitriser les impacts.</t>
+  </si>
+  <si>
+    <t>Suivi des versions</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Détail</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Première version validée pour diffusion publique</t>
+  </si>
+  <si>
+    <t>Roadmap</t>
+  </si>
+  <si>
+    <t>Les prochaines versions intégreront :</t>
+  </si>
+  <si>
+    <t>Les actions de niveau avancé</t>
+  </si>
+  <si>
+    <t>Les actions récurrentes</t>
+  </si>
+  <si>
+    <t>Une bibliothèque de contenus (définitions, kit de sensibilisation, …)</t>
+  </si>
+  <si>
+    <t>Vigilances</t>
+  </si>
+  <si>
+    <t>Il est fortement conseillé de dupliquer ce template dans un environnement maîtrisé, du fait de la sensibilité des données qu’il peut contenir une fois complété.</t>
+  </si>
+  <si>
+    <t>Lorsque des outils ou des solutions sont mentionnés, il ne s’agira que d’exemple, aucunement d’obligation.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">En aucun cas </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B for Security</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se porte garant de la bonne intégration des outils dans votre entité, ni de l’adéquation par rapport au besoin.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">En aucun cas </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B for Security</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se porte garant de l’impact de la mise en oeuvre de ces actions.</t>
+    </r>
+  </si>
+  <si>
+    <t>L’implémentation de ces actions ne vous garantit pas la protection totale contre un risque cybersécurité et des impacts associés.</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Prendre un RDV</t>
+  </si>
+  <si>
+    <t>Laisser un message vocal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -492,8 +685,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +882,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -835,7 +1050,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -861,6 +1076,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -907,14 +1142,194 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="173">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="217">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -926,27 +1341,50 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -958,27 +1396,50 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -990,24 +1451,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1019,24 +1462,91 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1048,24 +1558,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1077,16 +1569,37 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1097,6 +1610,214 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1117,358 +1838,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1484,20 +1853,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{92DD8A0B-6079-C04D-8683-83D370EDC52F}" name="Tableau0" displayName="Tableau0" ref="A1:G11" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{92DD8A0B-6079-C04D-8683-83D370EDC52F}" name="Tableau0" displayName="Tableau0" ref="A1:G11" totalsRowShown="0" headerRowDxfId="216" dataDxfId="215">
   <autoFilter ref="A1:G11" xr:uid="{92DD8A0B-6079-C04D-8683-83D370EDC52F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9F1B73B2-205E-FE46-A649-68E0274987D6}" name="ID" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{14B07E25-5ACF-764C-BF4E-0DDF061BCC32}" name="Objectifs" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{BB000758-931B-3A49-B35B-F2BEC84EDC93}" name="Précisions" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{F94AF8FF-ED3F-8A48-8CD0-A9C1A5A04367}" name="Onglet" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{BDBA1E0C-7E68-5142-88FC-A59E5044D401}" name="Etat" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{9F1B73B2-205E-FE46-A649-68E0274987D6}" name="ID" dataDxfId="214"/>
+    <tableColumn id="2" xr3:uid="{14B07E25-5ACF-764C-BF4E-0DDF061BCC32}" name="Objectifs" dataDxfId="213"/>
+    <tableColumn id="3" xr3:uid="{BB000758-931B-3A49-B35B-F2BEC84EDC93}" name="Précisions" dataDxfId="212"/>
+    <tableColumn id="4" xr3:uid="{F94AF8FF-ED3F-8A48-8CD0-A9C1A5A04367}" name="Onglet" dataDxfId="211"/>
+    <tableColumn id="5" xr3:uid="{BDBA1E0C-7E68-5142-88FC-A59E5044D401}" name="Etat" dataDxfId="210">
       <calculatedColumnFormula>IF(COUNTIF(Tableau1[Etat],"Terminé")=5,"Terminé",IF(COUNTIF(Tableau1[Etat],"A faire")=5,"A faire","En cours"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7F369ED5-32D5-1A4B-A7B4-2FDABDB4C4EE}" name="Date de début" dataDxfId="57">
+    <tableColumn id="6" xr3:uid="{7F369ED5-32D5-1A4B-A7B4-2FDABDB4C4EE}" name="Date de début" dataDxfId="209">
       <calculatedColumnFormula>IF(Tableau0[[#This Row],[Etat]]="En cours",MIN(Tableau10[Date de début]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DF3E834C-0481-5A48-A32E-1885D51E4CD2}" name="Date de clôture" dataDxfId="56">
+    <tableColumn id="8" xr3:uid="{DF3E834C-0481-5A48-A32E-1885D51E4CD2}" name="Date de clôture" dataDxfId="208">
       <calculatedColumnFormula>IF(Tableau0[[#This Row],[Etat]]="Terminé",MAX(Tableau7[Date de clôture]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1506,160 +1875,232 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B145B64-472B-2543-9135-FAC25A58BCF2}" name="Tableau9" displayName="Tableau9" ref="A1:G2" headerRowDxfId="12" dataDxfId="10" totalsRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B145B64-472B-2543-9135-FAC25A58BCF2}" name="Tableau9" displayName="Tableau9" ref="A1:G2" headerRowDxfId="77" dataDxfId="76" totalsRowDxfId="75">
   <autoFilter ref="A1:G2" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{22BFA6FF-954C-684A-9B36-2CFD8FE564C9}" name="ID" dataDxfId="19" totalsRowDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{C101F568-0EBC-B245-AF60-DF6381087233}" name="Action" dataDxfId="18" totalsRowDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{A793068A-0FB3-AA49-B479-0C57E54BD9AC}" name="Etat" dataDxfId="17" totalsRowDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{97F695FE-ACD0-F24F-99D0-1D9F6731284F}" name="Précisions" dataDxfId="16" totalsRowDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{FDB93F75-3058-D748-8B9E-35B211A0CE4C}" name="Type action" dataDxfId="15" totalsRowDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{1827AB54-2813-F443-951F-9D06BD06563D}" name="Date de début" dataDxfId="14" totalsRowDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{6B4734E4-A1C3-B441-9A87-B969EFB14F46}" name="Date de clôture" dataDxfId="13" totalsRowDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{22BFA6FF-954C-684A-9B36-2CFD8FE564C9}" name="ID" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{C101F568-0EBC-B245-AF60-DF6381087233}" name="Action" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{A793068A-0FB3-AA49-B479-0C57E54BD9AC}" name="Etat" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{97F695FE-ACD0-F24F-99D0-1D9F6731284F}" name="Précisions" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{FDB93F75-3058-D748-8B9E-35B211A0CE4C}" name="Type action" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{1827AB54-2813-F443-951F-9D06BD06563D}" name="Date de début" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{6B4734E4-A1C3-B441-9A87-B969EFB14F46}" name="Date de clôture" dataDxfId="62" totalsRowDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3F705EAC-68C1-7C40-A191-C42A00E612FA}" name="Tableau10" displayName="Tableau10" ref="A1:G3" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3F705EAC-68C1-7C40-A191-C42A00E612FA}" name="Tableau10" displayName="Tableau10" ref="A1:G3" headerRowDxfId="60" dataDxfId="59" totalsRowDxfId="58">
   <autoFilter ref="A1:G3" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5DB5C2D7-0598-394B-8E4F-145D21275750}" name="ID" dataDxfId="9" totalsRowDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{553B7FE2-B2A5-264D-A705-BE6D3FFB49E6}" name="Action" dataDxfId="8" totalsRowDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{A1BFA70D-1C9A-E447-B072-471DEB7852F6}" name="Etat" dataDxfId="7" totalsRowDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{00D52346-45B4-174F-8CB1-58A176AE4759}" name="Précisions" dataDxfId="6" totalsRowDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{C96166C9-6E73-B246-8719-15B3DA615E8D}" name="Type action" dataDxfId="5" totalsRowDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{B23CA891-6BD8-604D-B796-048ABE84DBA1}" name="Date de début" dataDxfId="4" totalsRowDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{398D4A0E-3FB6-084C-854E-326C591C9E13}" name="Date de clôture" dataDxfId="3" totalsRowDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{5DB5C2D7-0598-394B-8E4F-145D21275750}" name="ID" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{553B7FE2-B2A5-264D-A705-BE6D3FFB49E6}" name="Action" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{A1BFA70D-1C9A-E447-B072-471DEB7852F6}" name="Etat" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{00D52346-45B4-174F-8CB1-58A176AE4759}" name="Précisions" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{C96166C9-6E73-B246-8719-15B3DA615E8D}" name="Type action" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{B23CA891-6BD8-604D-B796-048ABE84DBA1}" name="Date de début" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{398D4A0E-3FB6-084C-854E-326C591C9E13}" name="Date de clôture" dataDxfId="45" totalsRowDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F614D5F0-8D8F-124E-8579-2B1644F5B378}" name="Tableau11" displayName="Tableau11" ref="A13:H22" totalsRowShown="0" headerRowDxfId="43" dataDxfId="10">
+  <autoFilter ref="A13:H22" xr:uid="{F614D5F0-8D8F-124E-8579-2B1644F5B378}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{45558F72-6B2B-304F-B596-B02ECC129ED3}" name="MATERIEL" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{83A9F371-7457-7444-BA0F-C3B0D3D4D773}" name="Description" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{A794C23E-1CDE-1F44-899A-C2A87A57771B}" name="Système d'exploitation" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{1C5D436D-FE04-8540-8893-B176D2D6EF08}" name="Entités tierces liées" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{9F1BC110-92B1-FE42-978D-304731A1E1DB}" name="Logiciels liés" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{24F917C8-77A5-4846-A8C1-85A5B25677AA}" name="Règles de sauvegarde" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{E56ADF88-A85D-1840-827F-26B3FEB83ECD}" name="Support/Maintenance/Garantie" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{77AB9CD0-FBA1-874E-A9E1-AD735B88505E}" name="Données chiffrées" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{0329E94E-344D-F143-93DF-7B738287E70B}" name="Tableau1114" displayName="Tableau1114" ref="A1:O10" totalsRowShown="0" headerRowDxfId="42" dataDxfId="19">
+  <autoFilter ref="A1:O10" xr:uid="{0329E94E-344D-F143-93DF-7B738287E70B}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{07FC1937-D3EB-AA46-8BF4-DA99464EDAE3}" name="LOGICIEL" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{DCA57FA6-64EA-2B47-B4B9-17C242F8C4E1}" name="Description" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{EE9A0B54-32D0-334B-9E6E-C16230DF093C}" name="Localisation" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{DF58ADED-96F8-4A4B-8182-DBCF0E96D2CD}" name="Version" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{833E6B53-F65B-9044-AE8C-3C5EABACCC71}" name="Licence" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{1CC0BEA7-03C3-D941-9AE3-CE7D25861B17}" name="Sensible" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{A7982BC8-33BC-AB46-B9D1-35557A8033E5}" name="Support/Maintenance/Garantie" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{7D2B33D2-051D-7B44-870E-E2C1BB1F6894}" name="Données chiffrées" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{5FE9C5B2-8A97-9744-A24D-1ED2F14E3E71}" name="Type d'authentification" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{9B831021-4EAF-4342-8F0E-4E4E5B4127B4}" name="Profil" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{A8BB1BE2-6359-B844-BD24-1CA0E362B358}" name="Matériel lié" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{6B688510-AB34-2B47-8EF1-EC9359A57C60}" name="Entités tierces liées" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{6E747AA2-48AE-B744-9380-B773834D1BA2}" name="Exigences de sécurité" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{FDD0CE26-1562-8346-9DE7-40E17767099B}" name="Règles de sauvegarde" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{E313AD0B-18F5-564A-A3A2-40F63E842521}" name="Mise à jour" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{699E75B9-499F-8442-A1F6-7D41E52790B7}" name="Tableau14" displayName="Tableau14" ref="A25:G33" totalsRowShown="0" headerRowDxfId="41" dataDxfId="35">
+  <autoFilter ref="A25:G33" xr:uid="{699E75B9-499F-8442-A1F6-7D41E52790B7}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{EAD6B09E-B764-8245-8608-D5FD4CCDAA45}" name="INTERCONNEXION" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{43FC1840-A09E-FF4A-BAA2-B06DB386C6B4}" name="Description" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{2D7F81F7-3339-6D41-8344-C8B336492381}" name="Source" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{C8F56523-76CD-B441-B8F5-BDAE4FB8694A}" name="Destination" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{30709A6D-D647-DD4B-8A98-2C94DCE2FA99}" name="Protocole" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{CC0BADF2-D172-F74B-B052-A20C2C1C9CD9}" name="Données sensibles" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{ECB1A310-5012-8F40-AA1D-66C7B337632B}" name="Données chiffrées" dataDxfId="36"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B7DA80AF-9648-8F4F-9A00-614381664C1F}" name="Tableau15" displayName="Tableau15" ref="A36:F42" totalsRowShown="0" headerRowDxfId="40" dataDxfId="4">
+  <autoFilter ref="A36:F42" xr:uid="{B7DA80AF-9648-8F4F-9A00-614381664C1F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7AD3D391-8758-C346-83D8-120A8453FEA3}" name="ENTITE TIERCE" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0D74F137-1812-5C4F-8792-CFD5A2B850CA}" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{4665C57D-5CFC-224E-8A03-85BBD5A24A8B}" name="Exigences de sécurité" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{70F28E0A-340C-BF44-8779-F7CC5A3E07C0}" name="ColoContact sécuriténne4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{79E32136-8EBD-5A42-B991-5600957D4DC2}" name="Matériel lié" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{E6654E82-C2E8-AD40-BCC6-95FD024D7F7F}" name="Logiciel lié" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}" name="Tableau1" displayName="Tableau1" ref="A1:G6" headerRowDxfId="171" dataDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}" name="Tableau1" displayName="Tableau1" ref="A1:G6" headerRowDxfId="207" dataDxfId="206">
   <autoFilter ref="A1:G6" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ACFC7BE0-E3DA-CF4B-8A1C-E4C3940F3B43}" name="ID" dataDxfId="170" totalsRowDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{31729F68-FFA8-DB4A-89BB-18183F26F6B5}" name="Action" dataDxfId="169" totalsRowDxfId="159"/>
-    <tableColumn id="3" xr3:uid="{7817D300-12B0-044F-B283-C67BEDFA9531}" name="Etat" dataDxfId="168" totalsRowDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{E2B91CC3-3B5F-414D-852B-37242D0B75BF}" name="Précisions" dataDxfId="167" totalsRowDxfId="161"/>
-    <tableColumn id="5" xr3:uid="{94913C42-C047-CE40-90A4-C1AB62D26B2F}" name="Type action" dataDxfId="166" totalsRowDxfId="162"/>
-    <tableColumn id="6" xr3:uid="{16AFA813-6F3D-4A41-A9E5-2C75F9D12CB9}" name="Date de début" dataDxfId="157" totalsRowDxfId="163"/>
-    <tableColumn id="8" xr3:uid="{348CC253-6D6E-F142-B24A-5C22951E8940}" name="Date de clôture" dataDxfId="165" totalsRowDxfId="164"/>
+    <tableColumn id="1" xr3:uid="{ACFC7BE0-E3DA-CF4B-8A1C-E4C3940F3B43}" name="ID" dataDxfId="205" totalsRowDxfId="204"/>
+    <tableColumn id="2" xr3:uid="{31729F68-FFA8-DB4A-89BB-18183F26F6B5}" name="Action" dataDxfId="203" totalsRowDxfId="202"/>
+    <tableColumn id="3" xr3:uid="{7817D300-12B0-044F-B283-C67BEDFA9531}" name="Etat" dataDxfId="201" totalsRowDxfId="200"/>
+    <tableColumn id="4" xr3:uid="{E2B91CC3-3B5F-414D-852B-37242D0B75BF}" name="Précisions" dataDxfId="199" totalsRowDxfId="198"/>
+    <tableColumn id="5" xr3:uid="{94913C42-C047-CE40-90A4-C1AB62D26B2F}" name="Type action" dataDxfId="197" totalsRowDxfId="196"/>
+    <tableColumn id="6" xr3:uid="{16AFA813-6F3D-4A41-A9E5-2C75F9D12CB9}" name="Date de début" dataDxfId="195" totalsRowDxfId="194"/>
+    <tableColumn id="8" xr3:uid="{348CC253-6D6E-F142-B24A-5C22951E8940}" name="Date de clôture" dataDxfId="193" totalsRowDxfId="192"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8843E0DD-B272-4740-8110-66ACE9526DA8}" name="Tableau2" displayName="Tableau2" ref="A1:G5" headerRowDxfId="156" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8843E0DD-B272-4740-8110-66ACE9526DA8}" name="Tableau2" displayName="Tableau2" ref="A1:G5" headerRowDxfId="191" dataDxfId="190">
   <autoFilter ref="A1:G5" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E936180B-C161-C64B-986A-5DD03CBD0F66}" name="ID" dataDxfId="55" totalsRowDxfId="155"/>
-    <tableColumn id="2" xr3:uid="{EA35535C-53C2-804C-A5DA-A4499E307316}" name="Action" dataDxfId="54" totalsRowDxfId="154"/>
-    <tableColumn id="3" xr3:uid="{0B5A0D27-E717-D249-92FF-E57407EE3790}" name="Etat" dataDxfId="53" totalsRowDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{D547C1B8-9433-1E41-B360-B2C34ACA447E}" name="Précisions" dataDxfId="52" totalsRowDxfId="152"/>
-    <tableColumn id="5" xr3:uid="{DFBA4126-6FC7-BD48-B18B-776E6CB19FB8}" name="Type action" dataDxfId="51" totalsRowDxfId="151"/>
-    <tableColumn id="6" xr3:uid="{ED9DDC42-1DC4-7646-9CF6-E8F976445C9F}" name="Date de début" dataDxfId="50" totalsRowDxfId="150"/>
-    <tableColumn id="8" xr3:uid="{73AD4E8A-CC1D-1747-A99C-7454742AFF5E}" name="Date de clôture" dataDxfId="49" totalsRowDxfId="149"/>
+    <tableColumn id="1" xr3:uid="{E936180B-C161-C64B-986A-5DD03CBD0F66}" name="ID" dataDxfId="189" totalsRowDxfId="188"/>
+    <tableColumn id="2" xr3:uid="{EA35535C-53C2-804C-A5DA-A4499E307316}" name="Action" dataDxfId="187" totalsRowDxfId="186"/>
+    <tableColumn id="3" xr3:uid="{0B5A0D27-E717-D249-92FF-E57407EE3790}" name="Etat" dataDxfId="185" totalsRowDxfId="184"/>
+    <tableColumn id="4" xr3:uid="{D547C1B8-9433-1E41-B360-B2C34ACA447E}" name="Précisions" dataDxfId="183" totalsRowDxfId="182"/>
+    <tableColumn id="5" xr3:uid="{DFBA4126-6FC7-BD48-B18B-776E6CB19FB8}" name="Type action" dataDxfId="181" totalsRowDxfId="180"/>
+    <tableColumn id="6" xr3:uid="{ED9DDC42-1DC4-7646-9CF6-E8F976445C9F}" name="Date de début" dataDxfId="179" totalsRowDxfId="178"/>
+    <tableColumn id="8" xr3:uid="{73AD4E8A-CC1D-1747-A99C-7454742AFF5E}" name="Date de clôture" dataDxfId="177" totalsRowDxfId="176"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{731072C5-6733-414C-8E52-A16CF29C3086}" name="Tableau3" displayName="Tableau3" ref="A1:G6" headerRowDxfId="148" dataDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{731072C5-6733-414C-8E52-A16CF29C3086}" name="Tableau3" displayName="Tableau3" ref="A1:G6" headerRowDxfId="175" dataDxfId="174">
   <autoFilter ref="A1:G6" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D7032955-1D0D-4341-90A4-722685A73304}" name="ID" dataDxfId="145" totalsRowDxfId="146"/>
-    <tableColumn id="2" xr3:uid="{6E67A8BC-65D3-CB44-8C32-E09847578757}" name="Action" dataDxfId="143" totalsRowDxfId="144"/>
-    <tableColumn id="3" xr3:uid="{ED12E05B-DA7C-2C43-A0F8-A2F0C5BA7C08}" name="Etat" dataDxfId="141" totalsRowDxfId="142"/>
-    <tableColumn id="4" xr3:uid="{7F2FC239-DEC1-E74F-9B99-7B961F073C40}" name="Précisions" dataDxfId="139" totalsRowDxfId="140"/>
-    <tableColumn id="5" xr3:uid="{A977F22A-BD03-1C49-9456-90AF021A2934}" name="Type action" dataDxfId="137" totalsRowDxfId="138"/>
-    <tableColumn id="6" xr3:uid="{A9EFE4DA-EEAF-D549-B214-328BEFBA8336}" name="Date de début" dataDxfId="135" totalsRowDxfId="136"/>
-    <tableColumn id="8" xr3:uid="{2AD3ADE6-2678-9A4F-AA70-272CFBFD76D0}" name="Date de clôture" dataDxfId="133" totalsRowDxfId="134"/>
+    <tableColumn id="1" xr3:uid="{D7032955-1D0D-4341-90A4-722685A73304}" name="ID" dataDxfId="173" totalsRowDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{6E67A8BC-65D3-CB44-8C32-E09847578757}" name="Action" dataDxfId="171" totalsRowDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{ED12E05B-DA7C-2C43-A0F8-A2F0C5BA7C08}" name="Etat" dataDxfId="169" totalsRowDxfId="168"/>
+    <tableColumn id="4" xr3:uid="{7F2FC239-DEC1-E74F-9B99-7B961F073C40}" name="Précisions" dataDxfId="167" totalsRowDxfId="166"/>
+    <tableColumn id="5" xr3:uid="{A977F22A-BD03-1C49-9456-90AF021A2934}" name="Type action" dataDxfId="165" totalsRowDxfId="164"/>
+    <tableColumn id="6" xr3:uid="{A9EFE4DA-EEAF-D549-B214-328BEFBA8336}" name="Date de début" dataDxfId="163" totalsRowDxfId="162"/>
+    <tableColumn id="8" xr3:uid="{2AD3ADE6-2678-9A4F-AA70-272CFBFD76D0}" name="Date de clôture" dataDxfId="161" totalsRowDxfId="160"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{39D5CA1D-38C5-354C-A930-1E6E5E7A7DAF}" name="Tableau4" displayName="Tableau4" ref="A1:G2" headerRowDxfId="132" dataDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{39D5CA1D-38C5-354C-A930-1E6E5E7A7DAF}" name="Tableau4" displayName="Tableau4" ref="A1:G2" headerRowDxfId="159" dataDxfId="158">
   <autoFilter ref="A1:G2" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{511D0148-7F01-5A42-9BB5-4D33525A4BB6}" name="ID" dataDxfId="129" totalsRowDxfId="130"/>
-    <tableColumn id="2" xr3:uid="{76138ADA-7545-9841-8281-A41CC9D89560}" name="Action" dataDxfId="127" totalsRowDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{49C12463-4C3A-DB48-A971-63838A0DF4FA}" name="Etat" dataDxfId="125" totalsRowDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{B2DAF9EA-8366-9E4B-BF96-56004474C8DE}" name="Précisions" dataDxfId="123" totalsRowDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{736C39F1-5633-684A-A566-2DC9EB64EB56}" name="Type action" dataDxfId="121" totalsRowDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{A59DE2BC-2C16-3249-A9BA-7AE1EBBF4E3A}" name="Date de début" dataDxfId="119" totalsRowDxfId="120"/>
-    <tableColumn id="8" xr3:uid="{CD5E0ABB-3DA7-124F-A841-DDCDEFC68FC0}" name="Date de clôture" dataDxfId="117" totalsRowDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{511D0148-7F01-5A42-9BB5-4D33525A4BB6}" name="ID" dataDxfId="157" totalsRowDxfId="156"/>
+    <tableColumn id="2" xr3:uid="{76138ADA-7545-9841-8281-A41CC9D89560}" name="Action" dataDxfId="155" totalsRowDxfId="154"/>
+    <tableColumn id="3" xr3:uid="{49C12463-4C3A-DB48-A971-63838A0DF4FA}" name="Etat" dataDxfId="153" totalsRowDxfId="152"/>
+    <tableColumn id="4" xr3:uid="{B2DAF9EA-8366-9E4B-BF96-56004474C8DE}" name="Précisions" dataDxfId="151" totalsRowDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{736C39F1-5633-684A-A566-2DC9EB64EB56}" name="Type action" dataDxfId="149" totalsRowDxfId="148"/>
+    <tableColumn id="6" xr3:uid="{A59DE2BC-2C16-3249-A9BA-7AE1EBBF4E3A}" name="Date de début" dataDxfId="147" totalsRowDxfId="146"/>
+    <tableColumn id="8" xr3:uid="{CD5E0ABB-3DA7-124F-A841-DDCDEFC68FC0}" name="Date de clôture" dataDxfId="145" totalsRowDxfId="144"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4256C9DC-DBC0-1644-8B8E-4E1E04651B41}" name="Tableau5" displayName="Tableau5" ref="A1:G4" headerRowDxfId="116" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4256C9DC-DBC0-1644-8B8E-4E1E04651B41}" name="Tableau5" displayName="Tableau5" ref="A1:G4" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="A1:G4" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B4A0FD8D-586C-9744-A6FC-5F113B5254CC}" name="ID" dataDxfId="113" totalsRowDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{CC2CD355-0546-D340-A692-C5E677202F32}" name="Action" dataDxfId="111" totalsRowDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{BD7185DB-0F64-FF4E-92C1-2ABB3DFAB039}" name="Etat" dataDxfId="109" totalsRowDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{C31595A4-20D3-C54A-961E-B102845A9C8B}" name="Précisions" dataDxfId="107" totalsRowDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{2783A23E-7C22-234B-B52A-5657AEB2D4AF}" name="Type action" dataDxfId="105" totalsRowDxfId="106"/>
-    <tableColumn id="6" xr3:uid="{6978B673-74FC-2F4E-A726-E8FA9C7069ED}" name="Date de début" dataDxfId="103" totalsRowDxfId="104"/>
-    <tableColumn id="8" xr3:uid="{039D4DB6-63D8-D34D-83E9-72D74F6758CB}" name="Date de clôture" dataDxfId="101" totalsRowDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{B4A0FD8D-586C-9744-A6FC-5F113B5254CC}" name="ID" dataDxfId="141" totalsRowDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{CC2CD355-0546-D340-A692-C5E677202F32}" name="Action" dataDxfId="139" totalsRowDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{BD7185DB-0F64-FF4E-92C1-2ABB3DFAB039}" name="Etat" dataDxfId="137" totalsRowDxfId="136"/>
+    <tableColumn id="4" xr3:uid="{C31595A4-20D3-C54A-961E-B102845A9C8B}" name="Précisions" dataDxfId="135" totalsRowDxfId="134"/>
+    <tableColumn id="5" xr3:uid="{2783A23E-7C22-234B-B52A-5657AEB2D4AF}" name="Type action" dataDxfId="133" totalsRowDxfId="132"/>
+    <tableColumn id="6" xr3:uid="{6978B673-74FC-2F4E-A726-E8FA9C7069ED}" name="Date de début" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="8" xr3:uid="{039D4DB6-63D8-D34D-83E9-72D74F6758CB}" name="Date de clôture" dataDxfId="129" totalsRowDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7179C485-7C78-EF49-9512-8A9D861F161B}" name="Tableau6" displayName="Tableau6" ref="A1:G2" headerRowDxfId="40" dataDxfId="38" totalsRowDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7179C485-7C78-EF49-9512-8A9D861F161B}" name="Tableau6" displayName="Tableau6" ref="A1:G2" headerRowDxfId="127" dataDxfId="126" totalsRowDxfId="125">
   <autoFilter ref="A1:G2" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E0A719B0-7050-6E4D-9F2A-EB6B8259B34F}" name="ID" dataDxfId="47" totalsRowDxfId="100"/>
-    <tableColumn id="2" xr3:uid="{716E0769-C0F2-2E49-B472-8C8E4E6179B4}" name="Action" dataDxfId="46" totalsRowDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{EA4739D8-312A-9E45-B2BA-E8954D573ACC}" name="Etat" dataDxfId="45" totalsRowDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{E4DEC298-1E8D-D240-90E8-1C465A8183D5}" name="Précisions" dataDxfId="44" totalsRowDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{0A4EB8B7-91BA-6548-8C0E-E754B7EDCE55}" name="Type action" dataDxfId="43" totalsRowDxfId="96"/>
-    <tableColumn id="6" xr3:uid="{0B485016-672B-B540-9EE3-9E5604457CD2}" name="Date de début" dataDxfId="42" totalsRowDxfId="95"/>
-    <tableColumn id="8" xr3:uid="{1FCB28B6-2BA0-4045-B19E-2544A6F24A8C}" name="Date de clôture" dataDxfId="41" totalsRowDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{E0A719B0-7050-6E4D-9F2A-EB6B8259B34F}" name="ID" dataDxfId="124" totalsRowDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{716E0769-C0F2-2E49-B472-8C8E4E6179B4}" name="Action" dataDxfId="122" totalsRowDxfId="121"/>
+    <tableColumn id="3" xr3:uid="{EA4739D8-312A-9E45-B2BA-E8954D573ACC}" name="Etat" dataDxfId="120" totalsRowDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{E4DEC298-1E8D-D240-90E8-1C465A8183D5}" name="Précisions" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{0A4EB8B7-91BA-6548-8C0E-E754B7EDCE55}" name="Type action" dataDxfId="116" totalsRowDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{0B485016-672B-B540-9EE3-9E5604457CD2}" name="Date de début" dataDxfId="114" totalsRowDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{1FCB28B6-2BA0-4045-B19E-2544A6F24A8C}" name="Date de clôture" dataDxfId="112" totalsRowDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{04396DC2-649C-4E4F-8361-75FA83FF3BC9}" name="Tableau7" displayName="Tableau7" ref="A1:G2" headerRowDxfId="93" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{04396DC2-649C-4E4F-8361-75FA83FF3BC9}" name="Tableau7" displayName="Tableau7" ref="A1:G2" headerRowDxfId="110" dataDxfId="109">
   <autoFilter ref="A1:G2" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7874A2E1-DE9F-C045-A0EA-421B1DBAD731}" name="ID" dataDxfId="37" totalsRowDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{8EA8A18B-61D9-A247-86CD-37BE9B1F5114}" name="Action" dataDxfId="36" totalsRowDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{71483B0D-A1C6-2B4E-BD91-2DD2C9E458F3}" name="Etat" dataDxfId="35" totalsRowDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{47899284-E653-044F-8952-8D9D9D7BE623}" name="Précisions" dataDxfId="34" totalsRowDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{817866AF-33AB-B24D-BB74-829B50D35BED}" name="Type action" dataDxfId="33" totalsRowDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{F5150BF4-5D70-384D-9BA0-608E1C1846C9}" name="Date de début" dataDxfId="32" totalsRowDxfId="87"/>
-    <tableColumn id="8" xr3:uid="{3DB115B5-B7C8-7542-B5A4-DA076076FB91}" name="Date de clôture" dataDxfId="31" totalsRowDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{7874A2E1-DE9F-C045-A0EA-421B1DBAD731}" name="ID" dataDxfId="108" totalsRowDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{8EA8A18B-61D9-A247-86CD-37BE9B1F5114}" name="Action" dataDxfId="106" totalsRowDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{71483B0D-A1C6-2B4E-BD91-2DD2C9E458F3}" name="Etat" dataDxfId="104" totalsRowDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{47899284-E653-044F-8952-8D9D9D7BE623}" name="Précisions" dataDxfId="102" totalsRowDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{817866AF-33AB-B24D-BB74-829B50D35BED}" name="Type action" dataDxfId="100" totalsRowDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{F5150BF4-5D70-384D-9BA0-608E1C1846C9}" name="Date de début" dataDxfId="98" totalsRowDxfId="97"/>
+    <tableColumn id="8" xr3:uid="{3DB115B5-B7C8-7542-B5A4-DA076076FB91}" name="Date de clôture" dataDxfId="96" totalsRowDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{015049F3-C6AD-E244-941D-9E56A560A9E7}" name="Tableau8" displayName="Tableau8" ref="A1:G3" headerRowDxfId="22" dataDxfId="20" totalsRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{015049F3-C6AD-E244-941D-9E56A560A9E7}" name="Tableau8" displayName="Tableau8" ref="A1:G3" headerRowDxfId="94" dataDxfId="93" totalsRowDxfId="92">
   <autoFilter ref="A1:G3" xr:uid="{F93719CB-FA48-0042-ADF4-E159AF61544B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{410F4084-7D4F-2F40-96E0-31C49F39AE1E}" name="ID" dataDxfId="29" totalsRowDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{B3A2E706-7F25-D04F-B570-302418594CDD}" name="Action" dataDxfId="28" totalsRowDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{A029C110-8586-8347-96F8-F45F46203311}" name="Etat" dataDxfId="27" totalsRowDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{631A6653-3462-104D-B60F-5D33A8811EDA}" name="Précisions" dataDxfId="26" totalsRowDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{3E080835-F21E-8548-BC25-B2E968A28BFF}" name="Type action" dataDxfId="25" totalsRowDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{6FA8E475-F83C-814A-B2A3-432C5D20B526}" name="Date de début" dataDxfId="24" totalsRowDxfId="80"/>
-    <tableColumn id="8" xr3:uid="{B04431D2-B0CE-6740-9EB0-FBC5FE10480E}" name="Date de clôture" dataDxfId="23" totalsRowDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{410F4084-7D4F-2F40-96E0-31C49F39AE1E}" name="ID" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{B3A2E706-7F25-D04F-B570-302418594CDD}" name="Action" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{A029C110-8586-8347-96F8-F45F46203311}" name="Etat" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{631A6653-3462-104D-B60F-5D33A8811EDA}" name="Précisions" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{3E080835-F21E-8548-BC25-B2E968A28BFF}" name="Type action" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{6FA8E475-F83C-814A-B2A3-432C5D20B526}" name="Date de début" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{B04431D2-B0CE-6740-9EB0-FBC5FE10480E}" name="Date de clôture" dataDxfId="79" totalsRowDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1982,19 +2423,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0298069-FB07-D34E-9350-C27D043F0443}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A2:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="10.83203125" style="4"/>
-    <col min="6" max="7" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="1.1640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="11"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="5" width="10.83203125" style="11"/>
+    <col min="6" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="16384" width="10.83203125" style="11"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="2:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="17">
+        <v>45310</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="2:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="17" spans="2:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" display="https://outlook.office.com/bookwithme/user/d3d9d6326537434aa2759d7e8f0db31f@bforsecurity.fr/meetingtype/SVRwCe7HMUGxuT6WGxi68g2?anonymous&amp;ep=mcard" xr:uid="{3306C212-B8BA-1C48-B489-5FD2D90A304C}"/>
+    <hyperlink ref="B26" r:id="rId2" display="https://www.speakpipe.com/BforSecurity" xr:uid="{5DC508C9-A61A-3648-8BBF-F49573F93A71}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2252,15 +2834,552 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D6F1D3-3A82-3245-A0C1-2C7469A29D85}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="13.5" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="13" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="36" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H14:H22 H2:H10 F2:F10 M2:M10 F26:G34 C37:C42" xr:uid="{F20E85C5-CCA5-C841-8616-2E3915CECD11}">
+      <formula1>"Oui,Non"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{ACAE1C5E-0ABD-1B4F-81A3-05A829D4E291}">
+      <formula1>"Local,Serveur,SaaS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I10" xr:uid="{A85BCA93-AC9F-0C44-AD75-A1A2546015BC}">
+      <formula1>"Authentification forte, Login/MDP"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J10" xr:uid="{ADAFEF8C-0B8A-4449-B058-63932D0DCD63}">
+      <formula1>"Utilisateur,Privilège"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K10 E37:E42" xr:uid="{CF90792F-8968-C948-92E2-198DE5C2F90B}">
+      <formula1>$A$14:$A$22</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O10" xr:uid="{3C343443-478D-154E-92F7-43A21CF67A40}">
+      <formula1>"Automatique,Manuel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D22" xr:uid="{379CCE93-1E2E-0C44-B0EA-5968CB31BD37}">
+      <formula1>$A$37:$A$42</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14:E22 F37:F42" xr:uid="{889664A0-E4C6-7A4B-878A-9D8F6527115F}">
+      <formula1>$A$2:$A$10</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2594,9 +3713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF08B05-BC23-BD40-B810-099CB8F8A526}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>